<commit_message>
Addition of HR25 data from Huff Run volunteers and regraphing with these included data points.
</commit_message>
<xml_diff>
--- a/StormEvents.xlsx
+++ b/StormEvents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="400" windowWidth="25040" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -110,6 +111,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,7 +167,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -174,10 +176,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -516,7 +519,7 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +587,7 @@
       <c r="B2" s="5">
         <v>42923.499305555553</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="10">
         <v>6.4070000000000004E-3</v>
       </c>
       <c r="D2" s="3">
@@ -625,7 +628,7 @@
       <c r="B3" s="5">
         <v>42923.540972222225</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="10">
         <v>6.5050000000000004E-3</v>
       </c>
       <c r="D3" s="3">
@@ -666,7 +669,7 @@
       <c r="B4" s="5">
         <v>42923.582638946762</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="10">
         <v>1.3779E-2</v>
       </c>
       <c r="D4" s="3">
@@ -707,7 +710,7 @@
       <c r="B5" s="5">
         <v>42923.624305671299</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="10">
         <v>9.3620000000000005E-3</v>
       </c>
       <c r="D5" s="3">
@@ -748,7 +751,7 @@
       <c r="B6" s="5">
         <v>42923.665972395836</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <v>1.1135000000000001E-2</v>
       </c>
       <c r="D6" s="3">
@@ -789,7 +792,7 @@
       <c r="B7" s="5">
         <v>42923.707639120374</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="10">
         <v>8.3759999999999998E-3</v>
       </c>
       <c r="D7" s="3">
@@ -830,7 +833,7 @@
       <c r="B8" s="5">
         <v>42923.749305844911</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="10">
         <v>6.7359999999999998E-3</v>
       </c>
       <c r="D8" s="3">
@@ -871,7 +874,7 @@
       <c r="B9" s="5">
         <v>42923.790972569448</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="10">
         <v>6.3119999999999999E-3</v>
       </c>
       <c r="D9" s="3">
@@ -912,7 +915,7 @@
       <c r="B10" s="5">
         <v>42923.832639293978</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="10">
         <v>5.0559999999999997E-3</v>
       </c>
       <c r="D10" s="3">
@@ -953,7 +956,7 @@
       <c r="B11" s="5">
         <v>42923.874306018515</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="10">
         <v>5.2769999999999996E-3</v>
       </c>
       <c r="D11" s="3">
@@ -994,7 +997,7 @@
       <c r="B12" s="5">
         <v>42923.915972743052</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="10">
         <v>3.9020000000000001E-3</v>
       </c>
       <c r="D12" s="3">
@@ -1035,7 +1038,7 @@
       <c r="B13" s="5">
         <v>42923.95763946759</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="10">
         <v>3.6029999999999999E-3</v>
       </c>
       <c r="D13" s="3">
@@ -1076,7 +1079,7 @@
       <c r="B14" s="5">
         <v>42929.495138888888</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="10">
         <v>9.0910000000000001E-3</v>
       </c>
       <c r="D14" s="3">
@@ -1117,7 +1120,7 @@
       <c r="B15" s="5">
         <v>42929.536805555559</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="10">
         <v>8.0759999999999998E-3</v>
       </c>
       <c r="D15" s="3">
@@ -1158,7 +1161,7 @@
       <c r="B16" s="5">
         <v>42929.578472280089</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="10">
         <v>7.8519999999999996E-3</v>
       </c>
       <c r="D16" s="3">
@@ -1199,7 +1202,7 @@
       <c r="B17" s="5">
         <v>42929.620139004626</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="10">
         <v>7.7520000000000002E-3</v>
       </c>
       <c r="D17" s="3">
@@ -1240,7 +1243,7 @@
       <c r="B18" s="5">
         <v>42929.661805729163</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="10">
         <v>7.2769999999999996E-3</v>
       </c>
       <c r="D18" s="3">
@@ -1281,7 +1284,7 @@
       <c r="B19" s="5">
         <v>42929.703472453701</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="10">
         <v>6.4200000000000004E-3</v>
       </c>
       <c r="D19" s="3">
@@ -1322,7 +1325,7 @@
       <c r="B20" s="5">
         <v>42929.745139178238</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="10">
         <v>5.5149999999999999E-3</v>
       </c>
       <c r="D20" s="3">
@@ -1363,7 +1366,7 @@
       <c r="B21" s="5">
         <v>42929.786805902775</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="10">
         <v>5.7999999999999996E-3</v>
       </c>
       <c r="D21" s="3">
@@ -1404,7 +1407,7 @@
       <c r="B22" s="5">
         <v>42929.828472627312</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="10">
         <v>6.0920000000000002E-3</v>
       </c>
       <c r="D22" s="3">
@@ -1445,7 +1448,7 @@
       <c r="B23" s="5">
         <v>42929.87013935185</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="10">
         <v>5.463E-3</v>
       </c>
       <c r="D23" s="3">
@@ -1486,7 +1489,7 @@
       <c r="B24" s="5">
         <v>42929.911806076387</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="10">
         <v>4.8780000000000004E-3</v>
       </c>
       <c r="D24" s="3">
@@ -1527,7 +1530,7 @@
       <c r="B25" s="5">
         <v>42929.953472800924</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="10">
         <v>4.8120000000000003E-3</v>
       </c>
       <c r="D25" s="3">
@@ -1568,7 +1571,7 @@
       <c r="B26" s="5">
         <v>43016.75</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="10">
         <v>5.8370000000000002E-3</v>
       </c>
       <c r="D26" s="3">
@@ -1609,7 +1612,7 @@
       <c r="B27" s="5">
         <v>43016.8125</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="10">
         <v>5.4440000000000001E-3</v>
       </c>
       <c r="D27" s="3">
@@ -1650,7 +1653,7 @@
       <c r="B28" s="5">
         <v>43016.875</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="10">
         <v>5.3369999999999997E-3</v>
       </c>
       <c r="D28" s="3">
@@ -1691,7 +1694,7 @@
       <c r="B29" s="5">
         <v>43016.9375</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="10">
         <v>5.4720000000000003E-3</v>
       </c>
       <c r="D29" s="3">
@@ -1732,7 +1735,7 @@
       <c r="B30" s="5">
         <v>43017</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="10">
         <v>9.8160000000000001E-3</v>
       </c>
       <c r="D30" s="3">
@@ -1773,7 +1776,7 @@
       <c r="B31" s="5">
         <v>43017.0625</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="10">
         <v>8.1779999999999995E-3</v>
       </c>
       <c r="D31" s="3">
@@ -1814,7 +1817,7 @@
       <c r="B32" s="5">
         <v>43017.125</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="10">
         <v>9.1750000000000009E-3</v>
       </c>
       <c r="D32" s="3">
@@ -1855,7 +1858,7 @@
       <c r="B33" s="5">
         <v>43017.1875</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="10">
         <v>1.1134E-2</v>
       </c>
       <c r="D33" s="3">
@@ -1896,7 +1899,7 @@
       <c r="B34" s="5">
         <v>43017.25</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="10">
         <v>1.0932000000000001E-2</v>
       </c>
       <c r="D34" s="3">
@@ -1937,7 +1940,7 @@
       <c r="B35" s="5">
         <v>43017.3125</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="10">
         <v>1.0558E-2</v>
       </c>
       <c r="D35" s="3">
@@ -1978,7 +1981,7 @@
       <c r="B36" s="5">
         <v>43017.375</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="10">
         <v>1.0018000000000001E-2</v>
       </c>
       <c r="D36" s="3">
@@ -2019,7 +2022,7 @@
       <c r="B37" s="5">
         <v>43017.4375</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="10">
         <v>9.2219999999999993E-3</v>
       </c>
       <c r="D37" s="3">
@@ -2060,7 +2063,7 @@
       <c r="B38" s="5">
         <v>43019.126388888886</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="10">
         <v>2.598E-3</v>
       </c>
       <c r="D38" s="3">
@@ -2101,7 +2104,7 @@
       <c r="B39" s="5">
         <v>43019.168055555558</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="10">
         <v>2.1919999999999999E-3</v>
       </c>
       <c r="D39" s="3">
@@ -2142,7 +2145,7 @@
       <c r="B40" s="5">
         <v>43019.209722280095</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D40" s="3">
@@ -2183,7 +2186,7 @@
       <c r="B41" s="5">
         <v>43019.251389004632</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D41" s="3">
@@ -2224,7 +2227,7 @@
       <c r="B42" s="5">
         <v>43019.293055729169</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D42" s="3">
@@ -2265,7 +2268,7 @@
       <c r="B43" s="5">
         <v>43019.334722453706</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D43" s="3">
@@ -2306,7 +2309,7 @@
       <c r="B44" s="5">
         <v>43019.376389178244</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D44" s="3">
@@ -2347,7 +2350,7 @@
       <c r="B45" s="5">
         <v>43019.418055902781</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D45" s="3">
@@ -2388,7 +2391,7 @@
       <c r="B46" s="5">
         <v>43019.459722627318</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D46" s="3">
@@ -2429,7 +2432,7 @@
       <c r="B47" s="5">
         <v>43019.501389351855</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="10">
         <v>1.7849999999999999E-3</v>
       </c>
       <c r="D47" s="3">
@@ -2470,7 +2473,7 @@
       <c r="B48" s="5">
         <v>43019.543056076385</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="10">
         <v>1.6379999999999999E-3</v>
       </c>
       <c r="D48" s="3">
@@ -2511,7 +2514,7 @@
       <c r="B49" s="5">
         <v>43019.584722800922</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="10">
         <v>1.6379999999999999E-3</v>
       </c>
       <c r="D49" s="3">
@@ -2552,7 +2555,7 @@
       <c r="B50" s="6">
         <v>43054.688194444447</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="10">
         <v>8.5863090288729911E-3</v>
       </c>
       <c r="D50" s="3">
@@ -2593,7 +2596,7 @@
       <c r="B51" s="6">
         <v>43054.729861111111</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="10">
         <v>9.2971120112089415E-3</v>
       </c>
       <c r="D51" s="3">
@@ -2634,7 +2637,7 @@
       <c r="B52" s="6">
         <v>43054.771527777775</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="10">
         <v>9.9129928652458427E-3</v>
       </c>
       <c r="D52" s="3">
@@ -2675,7 +2678,7 @@
       <c r="B53" s="6">
         <v>43054.813194444447</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="10">
         <v>9.9163013248413645E-3</v>
       </c>
       <c r="D53" s="3">
@@ -2716,7 +2719,7 @@
       <c r="B54" s="6">
         <v>43054.854861111111</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="10">
         <v>9.7251778225502204E-3</v>
       </c>
       <c r="D54" s="3">
@@ -2757,7 +2760,7 @@
       <c r="B55" s="6">
         <v>43054.896527777775</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="10">
         <v>9.6612416022987604E-3</v>
       </c>
       <c r="D55" s="3">
@@ -2798,7 +2801,7 @@
       <c r="B56" s="6">
         <v>43054.938194444447</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="10">
         <v>9.7890005236558435E-3</v>
       </c>
       <c r="D56" s="3">
@@ -2839,7 +2842,7 @@
       <c r="B57" s="6">
         <v>43054.979861111111</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="10">
         <v>9.7890005236558435E-3</v>
       </c>
       <c r="D57" s="3">
@@ -2880,7 +2883,7 @@
       <c r="B58" s="6">
         <v>43055.021527777775</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="10">
         <v>1.0152573613820461E-2</v>
       </c>
       <c r="D58" s="3">
@@ -2921,7 +2924,7 @@
       <c r="B59" s="6">
         <v>43055.063194444447</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="10">
         <v>1.0086380474935461E-2</v>
       </c>
       <c r="D59" s="3">
@@ -2962,7 +2965,7 @@
       <c r="B60" s="6">
         <v>43055.104861111111</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="10">
         <v>1.0020069600692096E-2</v>
       </c>
       <c r="D60" s="3">
@@ -3003,7 +3006,7 @@
       <c r="B61" s="9">
         <v>43055.146527777775</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="10">
         <v>9.9536420325516128E-3</v>
       </c>
       <c r="D61" s="3">

</xml_diff>